<commit_message>
fixed roxana's analisis bivariado
</commit_message>
<xml_diff>
--- a/datos/roxana_DatosDllSocial.xlsx
+++ b/datos/roxana_DatosDllSocial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uninorte-my.sharepoint.com/personal/rmanes_uninorte_edu_co/Documents/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F12E32C8-9FA4-5441-89CC-3E94254AF14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{0613F98D-6BD6-4CEE-A68C-60774C9AA2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AE510EC-D062-4EA9-9F44-B37F9AA13911}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BF6773D0-09CF-4874-B3DE-58312F6A3E19}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$A$150</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,10 +69,10 @@
     <t>NivelA</t>
   </si>
   <si>
-    <t>AG_Pre</t>
+    <t>CG_Post</t>
   </si>
   <si>
-    <t>AG_Post</t>
+    <t>CG_Pre</t>
   </si>
 </sst>
 </file>
@@ -117,9 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,15 +438,15 @@
   <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="6" width="11.43359375" style="1"/>
+    <col min="4" max="6" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -459,13 +460,13 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -475,17 +476,17 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>4.5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>70.5</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>74.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -495,17 +496,17 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>4</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>82.3</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -515,17 +516,17 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>3.6</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>62.7</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>68.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -535,17 +536,17 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>4.8</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>75.400000000000006</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -555,17 +556,17 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>69.8</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>83.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -575,17 +576,17 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>3.7</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>70.599999999999994</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>68.599999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -595,17 +596,17 @@
       <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>82.4</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>74.7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -615,17 +616,17 @@
       <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>62.8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>83.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -635,17 +636,17 @@
       <c r="C10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>4.5</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>75.5</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>68.7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -655,17 +656,17 @@
       <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>69.900000000000006</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>74.8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -675,17 +676,17 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>3.7</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>70.7</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>83.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -695,17 +696,17 @@
       <c r="C13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>82.5</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>68.8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -715,17 +716,17 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>4.13</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>62.9</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -735,17 +736,17 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>3.8</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>75.599999999999994</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <v>83.4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -755,17 +756,17 @@
       <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <v>4.2</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="2">
         <v>69.099999999999994</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2">
         <v>68.900000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -775,17 +776,17 @@
       <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <v>4</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>70.8</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -795,17 +796,17 @@
       <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>4.1500000000000004</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <v>82.6</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="2">
         <v>83.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -815,17 +816,17 @@
       <c r="C19" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="2">
         <v>4.2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
         <v>62.1</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <v>68.099999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -835,17 +836,17 @@
       <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="2">
         <v>3.8</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="2">
         <v>75.7</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <v>74.11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -855,17 +856,17 @@
       <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <v>4.2</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="2">
         <v>69.11</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <v>83.6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -875,17 +876,17 @@
       <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>4.2699999999999996</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="2">
         <v>70.900000000000006</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="2">
         <v>68.11</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -895,17 +896,17 @@
       <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="2">
         <v>3.9</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="2">
         <v>82.7</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="2">
         <v>74.12</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -915,17 +916,17 @@
       <c r="C24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="2">
         <v>4.2</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="2">
         <v>62.11</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="2">
         <v>83.7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -935,17 +936,17 @@
       <c r="C25" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="2">
         <v>4.5</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="2">
         <v>75.8</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="2">
         <v>68.12</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -955,17 +956,17 @@
       <c r="C26" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="2">
         <v>69.12</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="2">
         <v>74.13</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -975,17 +976,17 @@
       <c r="C27" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="2">
         <v>3.7</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="2">
         <v>70.099999999999994</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="2">
         <v>83.8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -995,17 +996,17 @@
       <c r="C28" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="2">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="2">
         <v>82.8</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="2">
         <v>68.13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1015,17 +1016,17 @@
       <c r="C29" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="2">
         <v>4.13</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="2">
         <v>62.12</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="2">
         <v>74.14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1035,17 +1036,17 @@
       <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="2">
         <v>3.8</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="2">
         <v>75.900000000000006</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="2">
         <v>83.9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1055,17 +1056,17 @@
       <c r="C31" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="2">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="2">
         <v>69.13</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="2">
         <v>68.14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1075,17 +1076,17 @@
       <c r="C32" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="2">
         <v>70.11</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="2">
         <v>74.150000000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1095,17 +1096,17 @@
       <c r="C33" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="2">
         <v>4.28</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="2">
         <v>70.099999999999994</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="2">
         <v>68.12</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1115,17 +1116,17 @@
       <c r="C34" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="2">
         <v>3.1</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="2">
         <v>82.8</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="2">
         <v>74.13</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1135,17 +1136,17 @@
       <c r="C35" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="2">
         <v>4.2</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="2">
         <v>62.12</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="2">
         <v>83.8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1155,17 +1156,17 @@
       <c r="C36" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="2">
         <v>4.5</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="2">
         <v>75.900000000000006</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="2">
         <v>68.13</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -1175,17 +1176,17 @@
       <c r="C37" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="2">
         <v>69.13</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="2">
         <v>74.14</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -1195,17 +1196,17 @@
       <c r="C38" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="2">
         <v>3.8</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2">
         <v>70.11</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="2">
         <v>83.9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1215,17 +1216,17 @@
       <c r="C39" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="2">
         <v>4.2</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="2">
         <v>82.9</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="2">
         <v>68.14</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -1235,17 +1236,17 @@
       <c r="C40" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="2">
         <v>4.2699999999999996</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="2">
         <v>62.13</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="2">
         <v>74.150000000000006</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -1255,17 +1256,17 @@
       <c r="C41" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="2">
         <v>3.9</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="2">
         <v>75.099999999999994</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="2">
         <v>83.1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1275,17 +1276,17 @@
       <c r="C42" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="2">
         <v>4.2</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="2">
         <v>69.14</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="2">
         <v>68.150000000000006</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1295,17 +1296,17 @@
       <c r="C43" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="2">
         <v>4</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="2">
         <v>70.12</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="2">
         <v>74.16</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1315,17 +1316,17 @@
       <c r="C44" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="2">
         <v>4.29</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="2">
         <v>70.11</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="2">
         <v>68.13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1335,17 +1336,17 @@
       <c r="C45" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="2">
         <v>3.11</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="2">
         <v>82.9</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="2">
         <v>74.14</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1355,17 +1356,17 @@
       <c r="C46" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="2">
         <v>4.2</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="2">
         <v>62.13</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="2">
         <v>83.9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -1375,17 +1376,17 @@
       <c r="C47" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="2">
         <v>4.5</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="2">
         <v>75.099999999999994</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="2">
         <v>68.14</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1395,17 +1396,17 @@
       <c r="C48" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="2">
         <v>69.14</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="2">
         <v>74.150000000000006</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -1415,17 +1416,17 @@
       <c r="C49" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="2">
         <v>3.9</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="2">
         <v>70.12</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="2">
         <v>83.1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -1435,17 +1436,17 @@
       <c r="C50" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="2">
         <v>4.34</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="2">
         <v>82.1</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="2">
         <v>68.150000000000006</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -1455,17 +1456,17 @@
       <c r="C51" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="2">
         <v>4.41</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="2">
         <v>62.14</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="2">
         <v>74.16</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -1475,17 +1476,17 @@
       <c r="C52" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="2">
         <v>3.1</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="2">
         <v>75.11</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="2">
         <v>83.11</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -1495,17 +1496,17 @@
       <c r="C53" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="2">
         <v>4.2</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="2">
         <v>69.150000000000006</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53" s="2">
         <v>68.16</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1515,17 +1516,17 @@
       <c r="C54" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="2">
         <v>70.13</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F54" s="2">
         <v>74.17</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -1535,17 +1536,17 @@
       <c r="C55" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="2">
         <v>4.3</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="2">
         <v>70.12</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="2">
         <v>68.14</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -1555,17 +1556,17 @@
       <c r="C56" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="2">
         <v>3.12</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="2">
         <v>82.1</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56" s="2">
         <v>74.150000000000006</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1575,17 +1576,17 @@
       <c r="C57" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="2">
         <v>4.2</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="2">
         <v>62.14</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57" s="2">
         <v>83.1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1595,17 +1596,17 @@
       <c r="C58" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="2">
         <v>4.5</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="2">
         <v>75.11</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F58" s="2">
         <v>68.150000000000006</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -1615,17 +1616,17 @@
       <c r="C59" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="2">
         <v>69.150000000000006</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="2">
         <v>74.16</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -1635,17 +1636,17 @@
       <c r="C60" t="s">
         <v>2</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="2">
         <v>3.1</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="2">
         <v>70.13</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60" s="2">
         <v>83.11</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -1655,17 +1656,17 @@
       <c r="C61" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="2">
         <v>4.4800000000000004</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="2">
         <v>82.11</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="2">
         <v>68.16</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -1675,17 +1676,17 @@
       <c r="C62" t="s">
         <v>3</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="2">
         <v>4.55</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="2">
         <v>62.15</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="2">
         <v>74.17</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -1695,17 +1696,17 @@
       <c r="C63" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="2">
         <v>3.11</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="2">
         <v>75.12</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="2">
         <v>83.12</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -1715,17 +1716,17 @@
       <c r="C64" t="s">
         <v>2</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="2">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="2">
         <v>69.16</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64" s="2">
         <v>68.17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -1735,17 +1736,17 @@
       <c r="C65" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="2">
         <v>4.8</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="2">
         <v>70.14</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="2">
         <v>74.180000000000007</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -1755,17 +1756,17 @@
       <c r="C66" t="s">
         <v>2</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="2">
         <v>4.3099999999999996</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="2">
         <v>70.13</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="2">
         <v>68.150000000000006</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -1775,17 +1776,17 @@
       <c r="C67" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="2">
         <v>3.13</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="2">
         <v>82.11</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67" s="2">
         <v>74.16</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -1795,17 +1796,17 @@
       <c r="C68" t="s">
         <v>2</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68" s="2">
         <v>4.2</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="2">
         <v>62.15</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68" s="2">
         <v>83.11</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -1815,17 +1816,17 @@
       <c r="C69" t="s">
         <v>3</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="2">
         <v>4.5</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="2">
         <v>75.12</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F69" s="2">
         <v>68.16</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -1835,17 +1836,17 @@
       <c r="C70" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="2">
         <v>69.16</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70" s="2">
         <v>74.17</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -1855,17 +1856,17 @@
       <c r="C71" t="s">
         <v>2</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="2">
         <v>3.11</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="2">
         <v>70.14</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F71" s="2">
         <v>83.12</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -1875,17 +1876,17 @@
       <c r="C72" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72" s="2">
         <v>4.62</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="2">
         <v>82.12</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72" s="2">
         <v>68.17</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -1895,17 +1896,17 @@
       <c r="C73" t="s">
         <v>3</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="2">
         <v>4.6900000000000004</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="2">
         <v>62.16</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73" s="2">
         <v>74.180000000000007</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -1915,17 +1916,17 @@
       <c r="C74" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="2">
         <v>3.12</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="2">
         <v>75.13</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74" s="2">
         <v>83.13</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -1935,17 +1936,17 @@
       <c r="C75" t="s">
         <v>2</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="2">
         <v>69.17</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F75" s="2">
         <v>68.180000000000007</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -1955,17 +1956,17 @@
       <c r="C76" t="s">
         <v>2</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="2">
         <v>4.12</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="2">
         <v>70.150000000000006</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F76" s="2">
         <v>74.19</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -1975,17 +1976,17 @@
       <c r="C77" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77" s="2">
         <v>4.32</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="2">
         <v>70.14</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F77" s="2">
         <v>68.16</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -1995,17 +1996,17 @@
       <c r="C78" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="2">
         <v>3.14</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="2">
         <v>82.12</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F78" s="2">
         <v>74.17</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -2015,17 +2016,17 @@
       <c r="C79" t="s">
         <v>2</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79" s="2">
         <v>4.2</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79" s="2">
         <v>62.16</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F79" s="2">
         <v>83.12</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -2035,17 +2036,17 @@
       <c r="C80" t="s">
         <v>3</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80" s="2">
         <v>4.5</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80" s="2">
         <v>75.13</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F80" s="2">
         <v>68.17</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -2055,17 +2056,17 @@
       <c r="C81" t="s">
         <v>2</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81" s="2">
         <v>69.17</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F81" s="2">
         <v>74.180000000000007</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -2075,17 +2076,17 @@
       <c r="C82" t="s">
         <v>2</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82" s="2">
         <v>3.12</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="2">
         <v>70.150000000000006</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F82" s="2">
         <v>83.13</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -2095,17 +2096,17 @@
       <c r="C83" t="s">
         <v>3</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83" s="2">
         <v>4.76</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="2">
         <v>82.13</v>
       </c>
-      <c r="F83" s="1">
+      <c r="F83" s="2">
         <v>68.180000000000007</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -2115,17 +2116,17 @@
       <c r="C84" t="s">
         <v>2</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D84" s="2">
         <v>4.83</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E84" s="2">
         <v>62.17</v>
       </c>
-      <c r="F84" s="1">
+      <c r="F84" s="2">
         <v>74.19</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -2135,17 +2136,17 @@
       <c r="C85" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="2">
         <v>3.13</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85" s="2">
         <v>75.14</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F85" s="2">
         <v>83.14</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -2155,17 +2156,17 @@
       <c r="C86" t="s">
         <v>2</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="2">
         <v>4.1399999999999997</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="2">
         <v>69.180000000000007</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F86" s="2">
         <v>68.19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -2175,17 +2176,17 @@
       <c r="C87" t="s">
         <v>2</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="2">
         <v>4.16</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87" s="2">
         <v>70.16</v>
       </c>
-      <c r="F87" s="1">
+      <c r="F87" s="2">
         <v>74.2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -2195,17 +2196,17 @@
       <c r="C88" t="s">
         <v>2</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D88" s="2">
         <v>4.33</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E88" s="2">
         <v>70.150000000000006</v>
       </c>
-      <c r="F88" s="1">
+      <c r="F88" s="2">
         <v>68.17</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -2215,17 +2216,17 @@
       <c r="C89" t="s">
         <v>3</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D89" s="2">
         <v>3.15</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E89" s="2">
         <v>82.13</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F89" s="2">
         <v>74.180000000000007</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -2235,17 +2236,17 @@
       <c r="C90" t="s">
         <v>2</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="2">
         <v>4.2</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E90" s="2">
         <v>62.17</v>
       </c>
-      <c r="F90" s="1">
+      <c r="F90" s="2">
         <v>83.13</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -2255,17 +2256,17 @@
       <c r="C91" t="s">
         <v>2</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D91" s="2">
         <v>4.5</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E91" s="2">
         <v>75.14</v>
       </c>
-      <c r="F91" s="1">
+      <c r="F91" s="2">
         <v>68.180000000000007</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -2275,17 +2276,17 @@
       <c r="C92" t="s">
         <v>2</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D92" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E92" s="2">
         <v>69.180000000000007</v>
       </c>
-      <c r="F92" s="1">
+      <c r="F92" s="2">
         <v>74.19</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -2295,17 +2296,17 @@
       <c r="C93" t="s">
         <v>2</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D93" s="2">
         <v>3.13</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E93" s="2">
         <v>70.16</v>
       </c>
-      <c r="F93" s="1">
+      <c r="F93" s="2">
         <v>83.14</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -2315,17 +2316,17 @@
       <c r="C94" t="s">
         <v>3</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D94" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E94" s="2">
         <v>82.14</v>
       </c>
-      <c r="F94" s="1">
+      <c r="F94" s="2">
         <v>68.19</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -2335,17 +2336,17 @@
       <c r="C95" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D95" s="2">
         <v>4.97</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E95" s="2">
         <v>62.18</v>
       </c>
-      <c r="F95" s="1">
+      <c r="F95" s="2">
         <v>74.2</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -2355,17 +2356,17 @@
       <c r="C96" t="s">
         <v>2</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96" s="2">
         <v>3.14</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="2">
         <v>75.150000000000006</v>
       </c>
-      <c r="F96" s="1">
+      <c r="F96" s="2">
         <v>83.15</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -2375,17 +2376,17 @@
       <c r="C97" t="s">
         <v>2</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D97" s="2">
         <v>4.18</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E97" s="2">
         <v>69.19</v>
       </c>
-      <c r="F97" s="1">
+      <c r="F97" s="2">
         <v>68.2</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -2395,17 +2396,17 @@
       <c r="C98" t="s">
         <v>2</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D98" s="2">
         <v>4.2</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E98" s="2">
         <v>70.17</v>
       </c>
-      <c r="F98" s="1">
+      <c r="F98" s="2">
         <v>74.209999999999994</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -2415,17 +2416,17 @@
       <c r="C99" t="s">
         <v>2</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99" s="2">
         <v>4.34</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E99" s="2">
         <v>70.16</v>
       </c>
-      <c r="F99" s="1">
+      <c r="F99" s="2">
         <v>68.180000000000007</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -2435,17 +2436,17 @@
       <c r="C100" t="s">
         <v>3</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D100" s="2">
         <v>3.16</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E100" s="2">
         <v>82.14</v>
       </c>
-      <c r="F100" s="1">
+      <c r="F100" s="2">
         <v>74.19</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -2455,17 +2456,17 @@
       <c r="C101" t="s">
         <v>2</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D101" s="2">
         <v>4.2</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E101" s="2">
         <v>62.18</v>
       </c>
-      <c r="F101" s="1">
+      <c r="F101" s="2">
         <v>83.14</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -2475,17 +2476,17 @@
       <c r="C102" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D102" s="2">
         <v>4.5</v>
       </c>
-      <c r="E102" s="1">
+      <c r="E102" s="2">
         <v>75.150000000000006</v>
       </c>
-      <c r="F102" s="1">
+      <c r="F102" s="2">
         <v>68.19</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -2495,17 +2496,17 @@
       <c r="C103" t="s">
         <v>2</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E103" s="1">
+      <c r="E103" s="2">
         <v>69.19</v>
       </c>
-      <c r="F103" s="1">
+      <c r="F103" s="2">
         <v>74.2</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -2515,17 +2516,17 @@
       <c r="C104" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104" s="2">
         <v>3.14</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E104" s="2">
         <v>70.17</v>
       </c>
-      <c r="F104" s="1">
+      <c r="F104" s="2">
         <v>83.15</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -2535,17 +2536,17 @@
       <c r="C105" t="s">
         <v>3</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105" s="2">
         <v>4.1040000000000001</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E105" s="2">
         <v>82.15</v>
       </c>
-      <c r="F105" s="1">
+      <c r="F105" s="2">
         <v>68.2</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1</v>
       </c>
@@ -2555,17 +2556,17 @@
       <c r="C106" t="s">
         <v>3</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106" s="2">
         <v>4.1109999999999998</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E106" s="2">
         <v>62.19</v>
       </c>
-      <c r="F106" s="1">
+      <c r="F106" s="2">
         <v>74.209999999999994</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1</v>
       </c>
@@ -2575,17 +2576,17 @@
       <c r="C107" t="s">
         <v>2</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107" s="2">
         <v>3.15</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E107" s="2">
         <v>75.16</v>
       </c>
-      <c r="F107" s="1">
+      <c r="F107" s="2">
         <v>83.16</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1</v>
       </c>
@@ -2595,17 +2596,17 @@
       <c r="C108" t="s">
         <v>2</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108" s="2">
         <v>4.22</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E108" s="2">
         <v>69.2</v>
       </c>
-      <c r="F108" s="1">
+      <c r="F108" s="2">
         <v>68.209999999999994</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -2615,17 +2616,17 @@
       <c r="C109" t="s">
         <v>2</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109" s="2">
         <v>4.24</v>
       </c>
-      <c r="E109" s="1">
+      <c r="E109" s="2">
         <v>70.180000000000007</v>
       </c>
-      <c r="F109" s="1">
+      <c r="F109" s="2">
         <v>74.22</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -2635,17 +2636,17 @@
       <c r="C110" t="s">
         <v>2</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110" s="2">
         <v>4.3499999999999996</v>
       </c>
-      <c r="E110" s="1">
+      <c r="E110" s="2">
         <v>70.17</v>
       </c>
-      <c r="F110" s="1">
+      <c r="F110" s="2">
         <v>68.19</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -2655,17 +2656,17 @@
       <c r="C111" t="s">
         <v>3</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111" s="2">
         <v>3.17</v>
       </c>
-      <c r="E111" s="1">
+      <c r="E111" s="2">
         <v>82.15</v>
       </c>
-      <c r="F111" s="1">
+      <c r="F111" s="2">
         <v>74.2</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -2675,17 +2676,17 @@
       <c r="C112" t="s">
         <v>2</v>
       </c>
-      <c r="D112" s="1">
+      <c r="D112" s="2">
         <v>4.2</v>
       </c>
-      <c r="E112" s="1">
+      <c r="E112" s="2">
         <v>62.19</v>
       </c>
-      <c r="F112" s="1">
+      <c r="F112" s="2">
         <v>83.15</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -2695,17 +2696,17 @@
       <c r="C113" t="s">
         <v>3</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113" s="2">
         <v>4.5</v>
       </c>
-      <c r="E113" s="1">
+      <c r="E113" s="2">
         <v>75.16</v>
       </c>
-      <c r="F113" s="1">
+      <c r="F113" s="2">
         <v>68.2</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -2715,17 +2716,17 @@
       <c r="C114" t="s">
         <v>2</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E114" s="2">
         <v>69.2</v>
       </c>
-      <c r="F114" s="1">
+      <c r="F114" s="2">
         <v>74.209999999999994</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -2735,17 +2736,17 @@
       <c r="C115" t="s">
         <v>2</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115" s="2">
         <v>3.15</v>
       </c>
-      <c r="E115" s="1">
+      <c r="E115" s="2">
         <v>70.180000000000007</v>
       </c>
-      <c r="F115" s="1">
+      <c r="F115" s="2">
         <v>83.16</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -2755,17 +2756,17 @@
       <c r="C116" t="s">
         <v>3</v>
       </c>
-      <c r="D116" s="1">
+      <c r="D116" s="2">
         <v>4.1180000000000003</v>
       </c>
-      <c r="E116" s="1">
+      <c r="E116" s="2">
         <v>82.16</v>
       </c>
-      <c r="F116" s="1">
+      <c r="F116" s="2">
         <v>68.209999999999994</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>1</v>
       </c>
@@ -2775,17 +2776,17 @@
       <c r="C117" t="s">
         <v>3</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D117" s="2">
         <v>4.125</v>
       </c>
-      <c r="E117" s="1">
+      <c r="E117" s="2">
         <v>62.2</v>
       </c>
-      <c r="F117" s="1">
+      <c r="F117" s="2">
         <v>74.22</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>1</v>
       </c>
@@ -2795,17 +2796,17 @@
       <c r="C118" t="s">
         <v>2</v>
       </c>
-      <c r="D118" s="1">
+      <c r="D118" s="2">
         <v>3.16</v>
       </c>
-      <c r="E118" s="1">
+      <c r="E118" s="2">
         <v>75.17</v>
       </c>
-      <c r="F118" s="1">
+      <c r="F118" s="2">
         <v>83.17</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>1</v>
       </c>
@@ -2815,17 +2816,17 @@
       <c r="C119" t="s">
         <v>2</v>
       </c>
-      <c r="D119" s="1">
+      <c r="D119" s="2">
         <v>4.26</v>
       </c>
-      <c r="E119" s="1">
+      <c r="E119" s="2">
         <v>69.209999999999994</v>
       </c>
-      <c r="F119" s="1">
+      <c r="F119" s="2">
         <v>68.22</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>1</v>
       </c>
@@ -2835,17 +2836,17 @@
       <c r="C120" t="s">
         <v>2</v>
       </c>
-      <c r="D120" s="1">
+      <c r="D120" s="2">
         <v>4.28</v>
       </c>
-      <c r="E120" s="1">
+      <c r="E120" s="2">
         <v>70.19</v>
       </c>
-      <c r="F120" s="1">
+      <c r="F120" s="2">
         <v>74.23</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>1</v>
       </c>
@@ -2855,17 +2856,17 @@
       <c r="C121" t="s">
         <v>2</v>
       </c>
-      <c r="D121" s="1">
+      <c r="D121" s="2">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E121" s="1">
+      <c r="E121" s="2">
         <v>70.180000000000007</v>
       </c>
-      <c r="F121" s="1">
+      <c r="F121" s="2">
         <v>68.2</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -2875,17 +2876,17 @@
       <c r="C122" t="s">
         <v>3</v>
       </c>
-      <c r="D122" s="1">
+      <c r="D122" s="2">
         <v>3.18</v>
       </c>
-      <c r="E122" s="1">
+      <c r="E122" s="2">
         <v>82.16</v>
       </c>
-      <c r="F122" s="1">
+      <c r="F122" s="2">
         <v>74.209999999999994</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1</v>
       </c>
@@ -2895,17 +2896,17 @@
       <c r="C123" t="s">
         <v>2</v>
       </c>
-      <c r="D123" s="1">
+      <c r="D123" s="2">
         <v>4.2</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E123" s="2">
         <v>62.2</v>
       </c>
-      <c r="F123" s="1">
+      <c r="F123" s="2">
         <v>83.16</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>1</v>
       </c>
@@ -2915,17 +2916,17 @@
       <c r="C124" t="s">
         <v>3</v>
       </c>
-      <c r="D124" s="1">
+      <c r="D124" s="2">
         <v>4.5</v>
       </c>
-      <c r="E124" s="1">
+      <c r="E124" s="2">
         <v>75.17</v>
       </c>
-      <c r="F124" s="1">
+      <c r="F124" s="2">
         <v>68.209999999999994</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>1</v>
       </c>
@@ -2935,17 +2936,17 @@
       <c r="C125" t="s">
         <v>2</v>
       </c>
-      <c r="D125" s="1">
+      <c r="D125" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E125" s="1">
+      <c r="E125" s="2">
         <v>69.209999999999994</v>
       </c>
-      <c r="F125" s="1">
+      <c r="F125" s="2">
         <v>74.22</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1</v>
       </c>
@@ -2955,17 +2956,17 @@
       <c r="C126" t="s">
         <v>2</v>
       </c>
-      <c r="D126" s="1">
+      <c r="D126" s="2">
         <v>3.16</v>
       </c>
-      <c r="E126" s="1">
+      <c r="E126" s="2">
         <v>70.19</v>
       </c>
-      <c r="F126" s="1">
+      <c r="F126" s="2">
         <v>83.17</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>1</v>
       </c>
@@ -2975,17 +2976,17 @@
       <c r="C127" t="s">
         <v>3</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D127" s="2">
         <v>4.1319999999999997</v>
       </c>
-      <c r="E127" s="1">
+      <c r="E127" s="2">
         <v>82.17</v>
       </c>
-      <c r="F127" s="1">
+      <c r="F127" s="2">
         <v>68.22</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>1</v>
       </c>
@@ -2995,17 +2996,17 @@
       <c r="C128" t="s">
         <v>3</v>
       </c>
-      <c r="D128" s="1">
+      <c r="D128" s="2">
         <v>4.1390000000000002</v>
       </c>
-      <c r="E128" s="1">
+      <c r="E128" s="2">
         <v>62.21</v>
       </c>
-      <c r="F128" s="1">
+      <c r="F128" s="2">
         <v>74.23</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1</v>
       </c>
@@ -3015,17 +3016,17 @@
       <c r="C129" t="s">
         <v>2</v>
       </c>
-      <c r="D129" s="1">
+      <c r="D129" s="2">
         <v>3.17</v>
       </c>
-      <c r="E129" s="1">
+      <c r="E129" s="2">
         <v>75.180000000000007</v>
       </c>
-      <c r="F129" s="1">
+      <c r="F129" s="2">
         <v>83.18</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>1</v>
       </c>
@@ -3035,17 +3036,17 @@
       <c r="C130" t="s">
         <v>2</v>
       </c>
-      <c r="D130" s="1">
+      <c r="D130" s="2">
         <v>4.3</v>
       </c>
-      <c r="E130" s="1">
+      <c r="E130" s="2">
         <v>69.22</v>
       </c>
-      <c r="F130" s="1">
+      <c r="F130" s="2">
         <v>68.23</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>1</v>
       </c>
@@ -3055,17 +3056,17 @@
       <c r="C131" t="s">
         <v>2</v>
       </c>
-      <c r="D131" s="1">
+      <c r="D131" s="2">
         <v>4.32</v>
       </c>
-      <c r="E131" s="1">
+      <c r="E131" s="2">
         <v>70.2</v>
       </c>
-      <c r="F131" s="1">
+      <c r="F131" s="2">
         <v>74.239999999999995</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>1</v>
       </c>
@@ -3075,17 +3076,17 @@
       <c r="C132" t="s">
         <v>2</v>
       </c>
-      <c r="D132" s="1">
+      <c r="D132" s="2">
         <v>4.37</v>
       </c>
-      <c r="E132" s="1">
+      <c r="E132" s="2">
         <v>70.19</v>
       </c>
-      <c r="F132" s="1">
+      <c r="F132" s="2">
         <v>68.209999999999994</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>1</v>
       </c>
@@ -3095,17 +3096,17 @@
       <c r="C133" t="s">
         <v>3</v>
       </c>
-      <c r="D133" s="1">
+      <c r="D133" s="2">
         <v>3.19</v>
       </c>
-      <c r="E133" s="1">
+      <c r="E133" s="2">
         <v>82.17</v>
       </c>
-      <c r="F133" s="1">
+      <c r="F133" s="2">
         <v>74.22</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -3115,17 +3116,17 @@
       <c r="C134" t="s">
         <v>2</v>
       </c>
-      <c r="D134" s="1">
+      <c r="D134" s="2">
         <v>4.2</v>
       </c>
-      <c r="E134" s="1">
+      <c r="E134" s="2">
         <v>62.21</v>
       </c>
-      <c r="F134" s="1">
+      <c r="F134" s="2">
         <v>83.17</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>1</v>
       </c>
@@ -3135,17 +3136,17 @@
       <c r="C135" t="s">
         <v>3</v>
       </c>
-      <c r="D135" s="1">
+      <c r="D135" s="2">
         <v>4.5</v>
       </c>
-      <c r="E135" s="1">
+      <c r="E135" s="2">
         <v>75.180000000000007</v>
       </c>
-      <c r="F135" s="1">
+      <c r="F135" s="2">
         <v>68.22</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>1</v>
       </c>
@@ -3155,17 +3156,17 @@
       <c r="C136" t="s">
         <v>2</v>
       </c>
-      <c r="D136" s="1">
+      <c r="D136" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E136" s="1">
+      <c r="E136" s="2">
         <v>69.22</v>
       </c>
-      <c r="F136" s="1">
+      <c r="F136" s="2">
         <v>74.23</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>1</v>
       </c>
@@ -3175,17 +3176,17 @@
       <c r="C137" t="s">
         <v>2</v>
       </c>
-      <c r="D137" s="1">
+      <c r="D137" s="2">
         <v>3.17</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137" s="2">
         <v>70.2</v>
       </c>
-      <c r="F137" s="1">
+      <c r="F137" s="2">
         <v>83.18</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>1</v>
       </c>
@@ -3195,17 +3196,17 @@
       <c r="C138" t="s">
         <v>3</v>
       </c>
-      <c r="D138" s="1">
+      <c r="D138" s="2">
         <v>4.1459999999999999</v>
       </c>
-      <c r="E138" s="1">
+      <c r="E138" s="2">
         <v>82.18</v>
       </c>
-      <c r="F138" s="1">
+      <c r="F138" s="2">
         <v>68.23</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>1</v>
       </c>
@@ -3215,17 +3216,17 @@
       <c r="C139" t="s">
         <v>3</v>
       </c>
-      <c r="D139" s="1">
+      <c r="D139" s="2">
         <v>4.1529999999999996</v>
       </c>
-      <c r="E139" s="1">
+      <c r="E139" s="2">
         <v>62.22</v>
       </c>
-      <c r="F139" s="1">
+      <c r="F139" s="2">
         <v>74.239999999999995</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>1</v>
       </c>
@@ -3235,17 +3236,17 @@
       <c r="C140" t="s">
         <v>2</v>
       </c>
-      <c r="D140" s="1">
+      <c r="D140" s="2">
         <v>3.18</v>
       </c>
-      <c r="E140" s="1">
+      <c r="E140" s="2">
         <v>75.19</v>
       </c>
-      <c r="F140" s="1">
+      <c r="F140" s="2">
         <v>83.19</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>1</v>
       </c>
@@ -3255,17 +3256,17 @@
       <c r="C141" t="s">
         <v>2</v>
       </c>
-      <c r="D141" s="1">
+      <c r="D141" s="2">
         <v>4.34</v>
       </c>
-      <c r="E141" s="1">
+      <c r="E141" s="2">
         <v>69.23</v>
       </c>
-      <c r="F141" s="1">
+      <c r="F141" s="2">
         <v>68.239999999999995</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>1</v>
       </c>
@@ -3275,17 +3276,17 @@
       <c r="C142" t="s">
         <v>2</v>
       </c>
-      <c r="D142" s="1">
+      <c r="D142" s="2">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E142" s="1">
+      <c r="E142" s="2">
         <v>70.209999999999994</v>
       </c>
-      <c r="F142" s="1">
+      <c r="F142" s="2">
         <v>74.25</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>1</v>
       </c>
@@ -3295,17 +3296,17 @@
       <c r="C143" t="s">
         <v>2</v>
       </c>
-      <c r="D143" s="1">
+      <c r="D143" s="2">
         <v>4.38</v>
       </c>
-      <c r="E143" s="1">
+      <c r="E143" s="2">
         <v>70.2</v>
       </c>
-      <c r="F143" s="1">
+      <c r="F143" s="2">
         <v>68.22</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>1</v>
       </c>
@@ -3315,17 +3316,17 @@
       <c r="C144" t="s">
         <v>3</v>
       </c>
-      <c r="D144" s="1">
+      <c r="D144" s="2">
         <v>3.2</v>
       </c>
-      <c r="E144" s="1">
+      <c r="E144" s="2">
         <v>82.18</v>
       </c>
-      <c r="F144" s="1">
+      <c r="F144" s="2">
         <v>74.23</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>1</v>
       </c>
@@ -3335,17 +3336,17 @@
       <c r="C145" t="s">
         <v>2</v>
       </c>
-      <c r="D145" s="1">
+      <c r="D145" s="2">
         <v>4.2</v>
       </c>
-      <c r="E145" s="1">
+      <c r="E145" s="2">
         <v>62.22</v>
       </c>
-      <c r="F145" s="1">
+      <c r="F145" s="2">
         <v>83.18</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>1</v>
       </c>
@@ -3355,17 +3356,17 @@
       <c r="C146" t="s">
         <v>3</v>
       </c>
-      <c r="D146" s="1">
+      <c r="D146" s="2">
         <v>4.5</v>
       </c>
-      <c r="E146" s="1">
+      <c r="E146" s="2">
         <v>75.19</v>
       </c>
-      <c r="F146" s="1">
+      <c r="F146" s="2">
         <v>68.23</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>1</v>
       </c>
@@ -3375,17 +3376,17 @@
       <c r="C147" t="s">
         <v>2</v>
       </c>
-      <c r="D147" s="1">
+      <c r="D147" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E147" s="1">
+      <c r="E147" s="2">
         <v>69.23</v>
       </c>
-      <c r="F147" s="1">
+      <c r="F147" s="2">
         <v>74.239999999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>1</v>
       </c>
@@ -3395,17 +3396,17 @@
       <c r="C148" t="s">
         <v>2</v>
       </c>
-      <c r="D148" s="1">
+      <c r="D148" s="2">
         <v>3.18</v>
       </c>
-      <c r="E148" s="1">
+      <c r="E148" s="2">
         <v>70.209999999999994</v>
       </c>
-      <c r="F148" s="1">
+      <c r="F148" s="2">
         <v>83.19</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>1</v>
       </c>
@@ -3415,17 +3416,17 @@
       <c r="C149" t="s">
         <v>3</v>
       </c>
-      <c r="D149" s="1">
+      <c r="D149" s="2">
         <v>4.16</v>
       </c>
-      <c r="E149" s="1">
+      <c r="E149" s="2">
         <v>82.19</v>
       </c>
-      <c r="F149" s="1">
+      <c r="F149" s="2">
         <v>68.239999999999995</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>1</v>
       </c>
@@ -3435,13 +3436,13 @@
       <c r="C150" t="s">
         <v>3</v>
       </c>
-      <c r="D150" s="1">
+      <c r="D150" s="2">
         <v>4.1669999999999998</v>
       </c>
-      <c r="E150" s="1">
+      <c r="E150" s="2">
         <v>62.23</v>
       </c>
-      <c r="F150" s="1">
+      <c r="F150" s="2">
         <v>74.25</v>
       </c>
     </row>

</xml_diff>